<commit_message>
Add requirements.txt and implement SUMMA algorithm with benchmarking for distributed matrix multiplication
</commit_message>
<xml_diff>
--- a/summa_fixed_value_benchmark_results.xlsx
+++ b/summa_fixed_value_benchmark_results.xlsx
@@ -450,7 +450,7 @@
         <v>500</v>
       </c>
       <c r="B2" t="n">
-        <v>0.7834937572479248</v>
+        <v>0.2240798473358154</v>
       </c>
     </row>
     <row r="3">
@@ -458,7 +458,7 @@
         <v>1000</v>
       </c>
       <c r="B3" t="n">
-        <v>0.7397902011871338</v>
+        <v>0.5015957355499268</v>
       </c>
     </row>
     <row r="4">
@@ -466,7 +466,7 @@
         <v>1500</v>
       </c>
       <c r="B4" t="n">
-        <v>1.369110345840454</v>
+        <v>1.568688631057739</v>
       </c>
     </row>
     <row r="5">
@@ -474,7 +474,7 @@
         <v>2000</v>
       </c>
       <c r="B5" t="n">
-        <v>3.219951629638672</v>
+        <v>3.871842622756958</v>
       </c>
     </row>
   </sheetData>

</xml_diff>